<commit_message>
prettify code + command line interaction
</commit_message>
<xml_diff>
--- a/Crawler/crawlresults.xlsx
+++ b/Crawler/crawlresults.xlsx
@@ -461,41 +461,41 @@
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
-          <t>Conflicted Features</t>
+          <t>Conflicting Features</t>
         </is>
       </c>
       <c r="G1" s="1" t="inlineStr">
         <is>
-          <t>Third Party Frames</t>
+          <t>Third Party Domains</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>https://permissionspolicy.xyz/</t>
+          <t>https://www.google.com/</t>
         </is>
       </c>
       <c r="B2" t="b">
         <v>1</v>
       </c>
       <c r="C2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E2" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>['geolocation']</t>
+          <t>[]</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>[['geolocation', 'permissionspolicy.cdn-gamma.com']]</t>
+          <t>[]</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
dataanalyzer and crawler can now work to add rows of crawled data
</commit_message>
<xml_diff>
--- a/Crawler/crawlresults.xlsx
+++ b/Crawler/crawlresults.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G2"/>
+  <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -473,27 +473,85 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>https://www.google.com/</t>
+          <t>https://permissionspolicy.xyz/</t>
         </is>
       </c>
       <c r="B2" t="b">
         <v>1</v>
       </c>
       <c r="C2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E2" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F2" t="inlineStr">
         <is>
+          <t>['geolocation']</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>['permissionspolicy.cdn-gamma.com']</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>https://google.com/</t>
+        </is>
+      </c>
+      <c r="B3" t="b">
+        <v>0</v>
+      </c>
+      <c r="C3" t="b">
+        <v>0</v>
+      </c>
+      <c r="D3" t="b">
+        <v>0</v>
+      </c>
+      <c r="E3" t="n">
+        <v>0</v>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
           <t>[]</t>
         </is>
       </c>
-      <c r="G2" t="inlineStr">
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>https://facebook.com/</t>
+        </is>
+      </c>
+      <c r="B4" t="b">
+        <v>0</v>
+      </c>
+      <c r="C4" t="b">
+        <v>0</v>
+      </c>
+      <c r="D4" t="b">
+        <v>0</v>
+      </c>
+      <c r="E4" t="n">
+        <v>0</v>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
         <is>
           <t>[]</t>
         </is>

</xml_diff>

<commit_message>
added more conditions, needs debugging
</commit_message>
<xml_diff>
--- a/Crawler/crawlresults.xlsx
+++ b/Crawler/crawlresults.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G4"/>
+  <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -473,36 +473,36 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>https://permissionspolicy.xyz/</t>
+          <t>https://google.com/</t>
         </is>
       </c>
       <c r="B2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E2" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>['geolocation']</t>
+          <t>[]</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>['permissionspolicy.cdn-gamma.com']</t>
+          <t>[]</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>https://google.com/</t>
+          <t>https://facebook.com/</t>
         </is>
       </c>
       <c r="B3" t="b">
@@ -523,35 +523,6 @@
         </is>
       </c>
       <c r="G3" t="inlineStr">
-        <is>
-          <t>[]</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>https://facebook.com/</t>
-        </is>
-      </c>
-      <c r="B4" t="b">
-        <v>0</v>
-      </c>
-      <c r="C4" t="b">
-        <v>0</v>
-      </c>
-      <c r="D4" t="b">
-        <v>0</v>
-      </c>
-      <c r="E4" t="n">
-        <v>0</v>
-      </c>
-      <c r="F4" t="inlineStr">
-        <is>
-          <t>[]</t>
-        </is>
-      </c>
-      <c r="G4" t="inlineStr">
         <is>
           <t>[]</t>
         </is>

</xml_diff>

<commit_message>
adding test applets to the rep
</commit_message>
<xml_diff>
--- a/Crawler/crawlresults.xlsx
+++ b/Crawler/crawlresults.xlsx
@@ -493,15 +493,15 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>https://www.vandale.nl/</t>
+          <t>https://www.jonglaan.nl/</t>
         </is>
       </c>
       <c r="B2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>[]</t>
+          <t>[('geolocation', ''), ('midi', ''), ('notifications', ''), ('push', ''), ('sync-xhr', ''), ('microphone', ''), ('camera', ''), ('magnetometer', ''), ('gyroscope', ''), ('speaker', 'self'), ('vibrate', ''), ('fullscreen', 'selfhttps://*.youtube.comhttps://*.youtube-nocookie.comhttps://*.youtu.be'), ('payment', '')]</t>
         </is>
       </c>
       <c r="D2" t="b">
@@ -509,12 +509,12 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
+          <t>[['microphone *', 'about:blank']]</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
           <t>[]</t>
-        </is>
-      </c>
-      <c r="F2" t="inlineStr">
-        <is>
-          <t>[['geolocation; microphone; camera; autoplay; fullscreen; payment; accelerometer; battery; ambient-light-sensor; display-capture; gyroscope; magnetometer; midi; ch-ua-platform-version; ch-ua-model'], ['geolocation; microphone; camera; autoplay; fullscreen; payment; accelerometer; battery; ambient-light-sensor; display-capture; gyroscope; magnetometer; midi; ch-ua-platform-version; ch-ua-model'], ['geolocation; microphone; camera; autoplay; fullscreen; payment; accelerometer; battery; ambient-light-sensor; display-capture; gyroscope; magnetometer; midi; ch-ua-platform-version; ch-ua-model']]</t>
         </is>
       </c>
       <c r="G2" t="b">
@@ -530,7 +530,7 @@
       </c>
       <c r="J2" t="inlineStr">
         <is>
-          <t>[]</t>
+          <t>['about:blank']</t>
         </is>
       </c>
       <c r="K2" t="b">

</xml_diff>